<commit_message>
Basic functionality without minor modifications
</commit_message>
<xml_diff>
--- a/excel_file.xlsx
+++ b/excel_file.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">Разработка ПО</t>
   </si>
   <si>
-    <t xml:space="preserve">Анализ требований; Написание кода</t>
+    <t xml:space="preserve">Анализ требований; Написание кода; kdshgjkdf</t>
   </si>
   <si>
     <t xml:space="preserve">Знание Python; Паттерны ООП</t>
@@ -119,6 +119,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -140,11 +141,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,15 +197,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -332,7 +335,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -369,7 +372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>